<commit_message>
actualización de asignación de aspirantes
</commit_message>
<xml_diff>
--- a/opciones educativas/resumen_asignacion.xlsx
+++ b/opciones educativas/resumen_asignacion.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="52">
   <si>
     <t xml:space="preserve">CVE_OPC</t>
   </si>
@@ -30,6 +30,9 @@
   </si>
   <si>
     <t xml:space="preserve">dif</t>
+  </si>
+  <si>
+    <t xml:space="preserve">asignados</t>
   </si>
   <si>
     <t xml:space="preserve">S054000</t>
@@ -515,13 +518,16 @@
       <c r="F1" t="s">
         <v>5</v>
       </c>
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B2" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C2" t="n">
         <v>334</v>
@@ -530,18 +536,21 @@
         <v>315</v>
       </c>
       <c r="E2" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="F2" t="n">
         <v>-19</v>
       </c>
+      <c r="G2" t="n">
+        <v>250</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B3" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C3" t="n">
         <v>401</v>
@@ -550,18 +559,21 @@
         <v>315</v>
       </c>
       <c r="E3" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="F3" t="n">
         <v>-86</v>
       </c>
+      <c r="G3" t="n">
+        <v>380</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B4" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C4" t="n">
         <v>205</v>
@@ -570,18 +582,21 @@
         <v>151</v>
       </c>
       <c r="E4" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="F4" t="n">
         <v>-54</v>
       </c>
+      <c r="G4" t="n">
+        <v>152</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B5" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C5" t="n">
         <v>150</v>
@@ -590,18 +605,21 @@
         <v>151</v>
       </c>
       <c r="E5" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="F5" t="n">
         <v>1</v>
       </c>
+      <c r="G5" t="n">
+        <v>150</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B6" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C6" t="n">
         <v>175</v>
@@ -610,18 +628,21 @@
         <v>200</v>
       </c>
       <c r="E6" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="F6" t="n">
         <v>25</v>
       </c>
+      <c r="G6" t="n">
+        <v>77</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B7" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C7" t="n">
         <v>458</v>
@@ -630,18 +651,21 @@
         <v>200</v>
       </c>
       <c r="E7" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="F7" t="n">
         <v>-258</v>
       </c>
+      <c r="G7" t="n">
+        <v>323</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B8" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C8" t="n">
         <v>55</v>
@@ -650,18 +674,21 @@
         <v>40</v>
       </c>
       <c r="E8" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="F8" t="n">
         <v>-15</v>
       </c>
+      <c r="G8" t="n">
+        <v>45</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B9" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C9" t="n">
         <v>36</v>
@@ -670,18 +697,21 @@
         <v>41</v>
       </c>
       <c r="E9" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="F9" t="n">
         <v>5</v>
       </c>
+      <c r="G9" t="n">
+        <v>36</v>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B10" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C10" t="n">
         <v>80</v>
@@ -690,18 +720,21 @@
         <v>42</v>
       </c>
       <c r="E10" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="F10" t="n">
         <v>-38</v>
       </c>
+      <c r="G10" t="n">
+        <v>73</v>
+      </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B11" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C11" t="n">
         <v>12</v>
@@ -710,18 +743,21 @@
         <v>43</v>
       </c>
       <c r="E11" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="F11" t="n">
         <v>31</v>
       </c>
+      <c r="G11" t="n">
+        <v>12</v>
+      </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B12" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C12" t="n">
         <v>161</v>
@@ -730,18 +766,21 @@
         <v>141</v>
       </c>
       <c r="E12" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="F12" t="n">
         <v>-20</v>
       </c>
+      <c r="G12" t="n">
+        <v>56</v>
+      </c>
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B13" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C13" t="n">
         <v>446</v>
@@ -750,18 +789,21 @@
         <v>142</v>
       </c>
       <c r="E13" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="F13" t="n">
         <v>-304</v>
       </c>
+      <c r="G13" t="n">
+        <v>227</v>
+      </c>
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B14" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C14" t="n">
         <v>88</v>
@@ -770,18 +812,21 @@
         <v>47</v>
       </c>
       <c r="E14" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="F14" t="n">
         <v>-41</v>
       </c>
+      <c r="G14" t="n">
+        <v>85</v>
+      </c>
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B15" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C15" t="n">
         <v>9</v>
@@ -790,18 +835,21 @@
         <v>47</v>
       </c>
       <c r="E15" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="F15" t="n">
         <v>38</v>
       </c>
+      <c r="G15" t="n">
+        <v>9</v>
+      </c>
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B16" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C16" t="n">
         <v>11</v>
@@ -810,18 +858,21 @@
         <v>30</v>
       </c>
       <c r="E16" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="F16" t="n">
         <v>19</v>
       </c>
+      <c r="G16" t="n">
+        <v>10</v>
+      </c>
     </row>
     <row r="17">
       <c r="A17" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B17" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C17" t="n">
         <v>52</v>
@@ -830,18 +881,21 @@
         <v>30</v>
       </c>
       <c r="E17" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="F17" t="n">
         <v>-22</v>
       </c>
+      <c r="G17" t="n">
+        <v>50</v>
+      </c>
     </row>
     <row r="18">
       <c r="A18" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B18" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C18" t="n">
         <v>40</v>
@@ -850,18 +904,21 @@
         <v>27</v>
       </c>
       <c r="E18" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="F18" t="n">
         <v>-13</v>
       </c>
+      <c r="G18" t="n">
+        <v>15</v>
+      </c>
     </row>
     <row r="19">
       <c r="A19" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B19" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C19" t="n">
         <v>48</v>
@@ -870,18 +927,21 @@
         <v>28</v>
       </c>
       <c r="E19" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="F19" t="n">
         <v>-20</v>
       </c>
+      <c r="G19" t="n">
+        <v>40</v>
+      </c>
     </row>
     <row r="20">
       <c r="A20" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B20" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C20" t="n">
         <v>114</v>
@@ -890,18 +950,21 @@
         <v>55</v>
       </c>
       <c r="E20" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="F20" t="n">
         <v>-59</v>
       </c>
+      <c r="G20" t="n">
+        <v>95</v>
+      </c>
     </row>
     <row r="21">
       <c r="A21" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B21" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C21" t="n">
         <v>15</v>
@@ -910,18 +973,21 @@
         <v>55</v>
       </c>
       <c r="E21" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="F21" t="n">
         <v>40</v>
       </c>
+      <c r="G21" t="n">
+        <v>15</v>
+      </c>
     </row>
     <row r="22">
       <c r="A22" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B22" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C22" t="n">
         <v>93</v>
@@ -930,18 +996,21 @@
         <v>105</v>
       </c>
       <c r="E22" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="F22" t="n">
         <v>12</v>
       </c>
+      <c r="G22" t="n">
+        <v>56</v>
+      </c>
     </row>
     <row r="23">
       <c r="A23" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B23" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C23" t="n">
         <v>205</v>
@@ -950,18 +1019,21 @@
         <v>105</v>
       </c>
       <c r="E23" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="F23" t="n">
         <v>-100</v>
       </c>
+      <c r="G23" t="n">
+        <v>154</v>
+      </c>
     </row>
     <row r="24">
       <c r="A24" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B24" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C24" t="n">
         <v>72</v>
@@ -970,18 +1042,21 @@
         <v>30</v>
       </c>
       <c r="E24" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="F24" t="n">
         <v>-42</v>
       </c>
+      <c r="G24" t="n">
+        <v>18</v>
+      </c>
     </row>
     <row r="25">
       <c r="A25" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B25" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C25" t="n">
         <v>61</v>
@@ -990,18 +1065,21 @@
         <v>30</v>
       </c>
       <c r="E25" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="F25" t="n">
         <v>-31</v>
       </c>
+      <c r="G25" t="n">
+        <v>42</v>
+      </c>
     </row>
     <row r="26">
       <c r="A26" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B26" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C26" t="n">
         <v>67</v>
@@ -1010,18 +1088,21 @@
         <v>122</v>
       </c>
       <c r="E26" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="F26" t="n">
         <v>55</v>
       </c>
+      <c r="G26" t="n">
+        <v>50</v>
+      </c>
     </row>
     <row r="27">
       <c r="A27" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B27" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C27" t="n">
         <v>216</v>
@@ -1030,18 +1111,21 @@
         <v>123</v>
       </c>
       <c r="E27" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="F27" t="n">
         <v>-93</v>
       </c>
+      <c r="G27" t="n">
+        <v>195</v>
+      </c>
     </row>
     <row r="28">
       <c r="A28" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B28" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C28" t="n">
         <v>61</v>
@@ -1050,18 +1134,21 @@
         <v>27</v>
       </c>
       <c r="E28" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="F28" t="n">
         <v>-34</v>
       </c>
+      <c r="G28" t="n">
+        <v>41</v>
+      </c>
     </row>
     <row r="29">
       <c r="A29" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B29" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C29" t="n">
         <v>14</v>
@@ -1070,18 +1157,21 @@
         <v>28</v>
       </c>
       <c r="E29" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="F29" t="n">
         <v>14</v>
       </c>
+      <c r="G29" t="n">
+        <v>14</v>
+      </c>
     </row>
     <row r="30">
       <c r="A30" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B30" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C30" t="n">
         <v>81</v>
@@ -1090,18 +1180,21 @@
         <v>87</v>
       </c>
       <c r="E30" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="F30" t="n">
         <v>6</v>
       </c>
+      <c r="G30" t="n">
+        <v>39</v>
+      </c>
     </row>
     <row r="31">
       <c r="A31" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B31" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C31" t="n">
         <v>226</v>
@@ -1110,18 +1203,21 @@
         <v>88</v>
       </c>
       <c r="E31" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="F31" t="n">
         <v>-138</v>
       </c>
+      <c r="G31" t="n">
+        <v>136</v>
+      </c>
     </row>
     <row r="32">
       <c r="A32" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B32" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C32" t="n">
         <v>62</v>
@@ -1130,18 +1226,21 @@
         <v>90</v>
       </c>
       <c r="E32" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="F32" t="n">
         <v>28</v>
       </c>
+      <c r="G32" t="n">
+        <v>33</v>
+      </c>
     </row>
     <row r="33">
       <c r="A33" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B33" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C33" t="n">
         <v>175</v>
@@ -1150,18 +1249,21 @@
         <v>90</v>
       </c>
       <c r="E33" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="F33" t="n">
         <v>-85</v>
       </c>
+      <c r="G33" t="n">
+        <v>147</v>
+      </c>
     </row>
     <row r="34">
       <c r="A34" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B34" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C34" t="n">
         <v>79</v>
@@ -1170,18 +1272,21 @@
         <v>60</v>
       </c>
       <c r="E34" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="F34" t="n">
         <v>-19</v>
       </c>
+      <c r="G34" t="n">
+        <v>51</v>
+      </c>
     </row>
     <row r="35">
       <c r="A35" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B35" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C35" t="n">
         <v>72</v>
@@ -1190,18 +1295,21 @@
         <v>60</v>
       </c>
       <c r="E35" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="F35" t="n">
         <v>-12</v>
       </c>
+      <c r="G35" t="n">
+        <v>69</v>
+      </c>
     </row>
     <row r="36">
       <c r="A36" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B36" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C36" t="n">
         <v>139</v>
@@ -1210,18 +1318,21 @@
         <v>90</v>
       </c>
       <c r="E36" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="F36" t="n">
         <v>-49</v>
       </c>
+      <c r="G36" t="n">
+        <v>119</v>
+      </c>
     </row>
     <row r="37">
       <c r="A37" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B37" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C37" t="n">
         <v>61</v>
@@ -1230,18 +1341,21 @@
         <v>90</v>
       </c>
       <c r="E37" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="F37" t="n">
         <v>29</v>
       </c>
+      <c r="G37" t="n">
+        <v>61</v>
+      </c>
     </row>
     <row r="38">
       <c r="A38" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B38" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C38" t="n">
         <v>144</v>
@@ -1250,18 +1364,21 @@
         <v>55</v>
       </c>
       <c r="E38" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="F38" t="n">
         <v>-89</v>
       </c>
+      <c r="G38" t="n">
+        <v>35</v>
+      </c>
     </row>
     <row r="39">
       <c r="A39" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B39" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C39" t="n">
         <v>166</v>
@@ -1270,18 +1387,21 @@
         <v>55</v>
       </c>
       <c r="E39" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="F39" t="n">
         <v>-111</v>
       </c>
+      <c r="G39" t="n">
+        <v>75</v>
+      </c>
     </row>
     <row r="40">
       <c r="A40" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B40" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C40" t="n">
         <v>65</v>
@@ -1290,18 +1410,21 @@
         <v>45</v>
       </c>
       <c r="E40" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="F40" t="n">
         <v>-20</v>
       </c>
+      <c r="G40" t="n">
+        <v>37</v>
+      </c>
     </row>
     <row r="41">
       <c r="A41" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B41" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C41" t="n">
         <v>58</v>
@@ -1310,18 +1433,21 @@
         <v>45</v>
       </c>
       <c r="E41" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="F41" t="n">
         <v>-13</v>
       </c>
+      <c r="G41" t="n">
+        <v>53</v>
+      </c>
     </row>
     <row r="42">
       <c r="A42" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B42" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C42" t="n">
         <v>67</v>
@@ -1330,18 +1456,21 @@
         <v>22</v>
       </c>
       <c r="E42" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="F42" t="n">
         <v>-45</v>
       </c>
+      <c r="G42" t="n">
+        <v>31</v>
+      </c>
     </row>
     <row r="43">
       <c r="A43" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B43" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C43" t="n">
         <v>14</v>
@@ -1350,18 +1479,21 @@
         <v>23</v>
       </c>
       <c r="E43" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="F43" t="n">
         <v>9</v>
+      </c>
+      <c r="G43" t="n">
+        <v>14</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B44" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C44" t="n">
         <v>29</v>
@@ -1370,18 +1502,21 @@
         <v>22</v>
       </c>
       <c r="E44" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="F44" t="n">
         <v>-7</v>
       </c>
+      <c r="G44" t="n">
+        <v>25</v>
+      </c>
     </row>
     <row r="45">
       <c r="A45" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B45" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C45" t="n">
         <v>20</v>
@@ -1390,18 +1525,21 @@
         <v>23</v>
       </c>
       <c r="E45" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="F45" t="n">
         <v>3</v>
       </c>
+      <c r="G45" t="n">
+        <v>20</v>
+      </c>
     </row>
     <row r="46">
       <c r="A46" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B46" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C46" t="n">
         <v>49</v>
@@ -1410,18 +1548,21 @@
         <v>22</v>
       </c>
       <c r="E46" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="F46" t="n">
         <v>-27</v>
       </c>
+      <c r="G46" t="n">
+        <v>18</v>
+      </c>
     </row>
     <row r="47">
       <c r="A47" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B47" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C47" t="n">
         <v>37</v>
@@ -1430,18 +1571,21 @@
         <v>23</v>
       </c>
       <c r="E47" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="F47" t="n">
         <v>-14</v>
       </c>
+      <c r="G47" t="n">
+        <v>27</v>
+      </c>
     </row>
     <row r="48">
       <c r="A48" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B48" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C48" t="n">
         <v>107</v>
@@ -1450,18 +1594,21 @@
         <v>45</v>
       </c>
       <c r="E48" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="F48" t="n">
         <v>-62</v>
       </c>
+      <c r="G48" t="n">
+        <v>44</v>
+      </c>
     </row>
     <row r="49">
       <c r="A49" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B49" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C49" t="n">
         <v>46</v>
@@ -1470,18 +1617,21 @@
         <v>45</v>
       </c>
       <c r="E49" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="F49" t="n">
         <v>-1</v>
       </c>
+      <c r="G49" t="n">
+        <v>46</v>
+      </c>
     </row>
     <row r="50">
       <c r="A50" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B50" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C50" t="n">
         <v>69</v>
@@ -1490,18 +1640,21 @@
         <v>45</v>
       </c>
       <c r="E50" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="F50" t="n">
         <v>-24</v>
       </c>
+      <c r="G50" t="n">
+        <v>51</v>
+      </c>
     </row>
     <row r="51">
       <c r="A51" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B51" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C51" t="n">
         <v>39</v>
@@ -1510,18 +1663,21 @@
         <v>45</v>
       </c>
       <c r="E51" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="F51" t="n">
         <v>6</v>
       </c>
+      <c r="G51" t="n">
+        <v>39</v>
+      </c>
     </row>
     <row r="52">
       <c r="A52" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B52" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C52" t="n">
         <v>50</v>
@@ -1530,18 +1686,21 @@
         <v>45</v>
       </c>
       <c r="E52" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="F52" t="n">
         <v>-5</v>
       </c>
+      <c r="G52" t="n">
+        <v>44</v>
+      </c>
     </row>
     <row r="53">
       <c r="A53" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B53" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C53" t="n">
         <v>46</v>
@@ -1550,18 +1709,21 @@
         <v>45</v>
       </c>
       <c r="E53" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="F53" t="n">
         <v>-1</v>
       </c>
+      <c r="G53" t="n">
+        <v>46</v>
+      </c>
     </row>
     <row r="54">
       <c r="A54" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B54" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C54" t="n">
         <v>137</v>
@@ -1570,18 +1732,21 @@
         <v>112</v>
       </c>
       <c r="E54" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="F54" t="n">
         <v>-25</v>
       </c>
+      <c r="G54" t="n">
+        <v>67</v>
+      </c>
     </row>
     <row r="55">
       <c r="A55" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B55" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C55" t="n">
         <v>208</v>
@@ -1590,18 +1755,21 @@
         <v>113</v>
       </c>
       <c r="E55" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="F55" t="n">
         <v>-95</v>
       </c>
+      <c r="G55" t="n">
+        <v>158</v>
+      </c>
     </row>
     <row r="56">
       <c r="A56" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B56" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C56" t="n">
         <v>127</v>
@@ -1610,18 +1778,21 @@
         <v>67</v>
       </c>
       <c r="E56" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="F56" t="n">
         <v>-60</v>
       </c>
+      <c r="G56" t="n">
+        <v>77</v>
+      </c>
     </row>
     <row r="57">
       <c r="A57" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B57" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C57" t="n">
         <v>58</v>
@@ -1630,18 +1801,21 @@
         <v>68</v>
       </c>
       <c r="E57" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="F57" t="n">
         <v>10</v>
+      </c>
+      <c r="G57" t="n">
+        <v>58</v>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B58" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C58" t="n">
         <v>163</v>
@@ -1650,18 +1824,21 @@
         <v>65</v>
       </c>
       <c r="E58" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="F58" t="n">
         <v>-98</v>
       </c>
+      <c r="G58" t="n">
+        <v>61</v>
+      </c>
     </row>
     <row r="59">
       <c r="A59" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B59" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C59" t="n">
         <v>74</v>
@@ -1670,18 +1847,21 @@
         <v>65</v>
       </c>
       <c r="E59" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="F59" t="n">
         <v>-9</v>
       </c>
+      <c r="G59" t="n">
+        <v>69</v>
+      </c>
     </row>
     <row r="60">
       <c r="A60" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B60" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C60" t="n">
         <v>240</v>
@@ -1690,18 +1870,21 @@
         <v>190</v>
       </c>
       <c r="E60" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="F60" t="n">
         <v>-50</v>
       </c>
+      <c r="G60" t="n">
+        <v>146</v>
+      </c>
     </row>
     <row r="61">
       <c r="A61" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B61" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C61" t="n">
         <v>268</v>
@@ -1710,18 +1893,21 @@
         <v>190</v>
       </c>
       <c r="E61" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="F61" t="n">
         <v>-78</v>
       </c>
+      <c r="G61" t="n">
+        <v>234</v>
+      </c>
     </row>
     <row r="62">
       <c r="A62" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B62" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C62" t="n">
         <v>84</v>
@@ -1730,18 +1916,21 @@
         <v>45</v>
       </c>
       <c r="E62" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="F62" t="n">
         <v>-39</v>
       </c>
+      <c r="G62" t="n">
+        <v>21</v>
+      </c>
     </row>
     <row r="63">
       <c r="A63" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B63" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C63" t="n">
         <v>190</v>
@@ -1750,18 +1939,21 @@
         <v>45</v>
       </c>
       <c r="E63" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="F63" t="n">
         <v>-145</v>
       </c>
+      <c r="G63" t="n">
+        <v>69</v>
+      </c>
     </row>
     <row r="64">
       <c r="A64" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B64" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C64" t="n">
         <v>166</v>
@@ -1770,18 +1962,21 @@
         <v>45</v>
       </c>
       <c r="E64" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="F64" t="n">
         <v>-121</v>
       </c>
+      <c r="G64" t="n">
+        <v>29</v>
+      </c>
     </row>
     <row r="65">
       <c r="A65" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B65" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C65" t="n">
         <v>160</v>
@@ -1790,18 +1985,21 @@
         <v>45</v>
       </c>
       <c r="E65" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="F65" t="n">
         <v>-115</v>
       </c>
+      <c r="G65" t="n">
+        <v>61</v>
+      </c>
     </row>
     <row r="66">
       <c r="A66" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B66" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C66" t="n">
         <v>157</v>
@@ -1810,18 +2008,21 @@
         <v>150</v>
       </c>
       <c r="E66" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="F66" t="n">
         <v>-7</v>
       </c>
+      <c r="G66" t="n">
+        <v>87</v>
+      </c>
     </row>
     <row r="67">
       <c r="A67" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B67" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C67" t="n">
         <v>272</v>
@@ -1830,18 +2031,21 @@
         <v>150</v>
       </c>
       <c r="E67" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="F67" t="n">
         <v>-122</v>
       </c>
+      <c r="G67" t="n">
+        <v>213</v>
+      </c>
     </row>
     <row r="68">
       <c r="A68" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B68" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C68" t="n">
         <v>45</v>
@@ -1850,18 +2054,21 @@
         <v>75</v>
       </c>
       <c r="E68" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="F68" t="n">
         <v>30</v>
       </c>
+      <c r="G68" t="n">
+        <v>43</v>
+      </c>
     </row>
     <row r="69">
       <c r="A69" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B69" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C69" t="n">
         <v>107</v>
@@ -1870,18 +2077,21 @@
         <v>75</v>
       </c>
       <c r="E69" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="F69" t="n">
         <v>-32</v>
       </c>
+      <c r="G69" t="n">
+        <v>107</v>
+      </c>
     </row>
     <row r="70">
       <c r="A70" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B70" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C70" t="n">
         <v>325</v>
@@ -1890,18 +2100,21 @@
         <v>107</v>
       </c>
       <c r="E70" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="F70" t="n">
         <v>-218</v>
       </c>
+      <c r="G70" t="n">
+        <v>65</v>
+      </c>
     </row>
     <row r="71">
       <c r="A71" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B71" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C71" t="n">
         <v>351</v>
@@ -1910,18 +2123,21 @@
         <v>108</v>
       </c>
       <c r="E71" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="F71" t="n">
         <v>-243</v>
       </c>
+      <c r="G71" t="n">
+        <v>150</v>
+      </c>
     </row>
     <row r="72">
       <c r="A72" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B72" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C72" t="n">
         <v>462</v>
@@ -1930,18 +2146,21 @@
         <v>175</v>
       </c>
       <c r="E72" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="F72" t="n">
         <v>-287</v>
       </c>
+      <c r="G72" t="n">
+        <v>92</v>
+      </c>
     </row>
     <row r="73">
       <c r="A73" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B73" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C73" t="n">
         <v>643</v>
@@ -1950,18 +2169,21 @@
         <v>175</v>
       </c>
       <c r="E73" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="F73" t="n">
         <v>-468</v>
       </c>
+      <c r="G73" t="n">
+        <v>258</v>
+      </c>
     </row>
     <row r="74">
       <c r="A74" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B74" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C74" t="n">
         <v>404</v>
@@ -1970,18 +2192,21 @@
         <v>250</v>
       </c>
       <c r="E74" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="F74" t="n">
         <v>-154</v>
       </c>
+      <c r="G74" t="n">
+        <v>139</v>
+      </c>
     </row>
     <row r="75">
       <c r="A75" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B75" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C75" t="n">
         <v>561</v>
@@ -1990,18 +2215,21 @@
         <v>250</v>
       </c>
       <c r="E75" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="F75" t="n">
         <v>-311</v>
       </c>
+      <c r="G75" t="n">
+        <v>361</v>
+      </c>
     </row>
     <row r="76">
       <c r="A76" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="B76" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C76" t="n">
         <v>194</v>
@@ -2010,18 +2238,21 @@
         <v>150</v>
       </c>
       <c r="E76" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="F76" t="n">
         <v>-44</v>
       </c>
+      <c r="G76" t="n">
+        <v>78</v>
+      </c>
     </row>
     <row r="77">
       <c r="A77" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="B77" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C77" t="n">
         <v>343</v>
@@ -2030,18 +2261,21 @@
         <v>150</v>
       </c>
       <c r="E77" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="F77" t="n">
         <v>-193</v>
       </c>
+      <c r="G77" t="n">
+        <v>222</v>
+      </c>
     </row>
     <row r="78">
       <c r="A78" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="B78" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C78" t="n">
         <v>172</v>
@@ -2050,18 +2284,21 @@
         <v>200</v>
       </c>
       <c r="E78" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="F78" t="n">
         <v>28</v>
       </c>
+      <c r="G78" t="n">
+        <v>136</v>
+      </c>
     </row>
     <row r="79">
       <c r="A79" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="B79" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C79" t="n">
         <v>273</v>
@@ -2070,18 +2307,21 @@
         <v>200</v>
       </c>
       <c r="E79" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="F79" t="n">
         <v>-73</v>
       </c>
+      <c r="G79" t="n">
+        <v>264</v>
+      </c>
     </row>
     <row r="80">
       <c r="A80" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="B80" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C80" t="n">
         <v>309</v>
@@ -2090,18 +2330,21 @@
         <v>325</v>
       </c>
       <c r="E80" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="F80" t="n">
         <v>16</v>
       </c>
+      <c r="G80" t="n">
+        <v>308</v>
+      </c>
     </row>
     <row r="81">
       <c r="A81" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="B81" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C81" t="n">
         <v>342</v>
@@ -2110,18 +2353,21 @@
         <v>325</v>
       </c>
       <c r="E81" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="F81" t="n">
         <v>-17</v>
       </c>
+      <c r="G81" t="n">
+        <v>342</v>
+      </c>
     </row>
     <row r="82">
       <c r="A82" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B82" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C82" t="n">
         <v>120</v>
@@ -2130,18 +2376,21 @@
         <v>100</v>
       </c>
       <c r="E82" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="F82" t="n">
         <v>-20</v>
       </c>
+      <c r="G82" t="n">
+        <v>59</v>
+      </c>
     </row>
     <row r="83">
       <c r="A83" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B83" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C83" t="n">
         <v>174</v>
@@ -2150,10 +2399,13 @@
         <v>100</v>
       </c>
       <c r="E83" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="F83" t="n">
         <v>-74</v>
+      </c>
+      <c r="G83" t="n">
+        <v>141</v>
       </c>
     </row>
   </sheetData>

</xml_diff>